<commit_message>
Atualização final pós feedback
</commit_message>
<xml_diff>
--- a/DOCUMENTAÇÃO/Backlog - Projeto-Individual.xlsx
+++ b/DOCUMENTAÇÃO/Backlog - Projeto-Individual.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matheus\Downloads\Projeto-Individual\DOCUMENTAÇÃO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{63E0B9FB-C5FF-492E-BCC7-B33538EE3227}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B41D7DE0-A61E-40F1-90E4-37A588CE0766}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="69">
   <si>
     <t>REQUISITOS PARA A PROJETO INDIVIDUAL - BACKLOG</t>
   </si>
@@ -80,9 +80,6 @@
     <t>ESSENCIAL</t>
   </si>
   <si>
-    <t>INCOMPLETO</t>
-  </si>
-  <si>
     <t>Planejamento</t>
   </si>
   <si>
@@ -246,9 +243,6 @@
   </si>
   <si>
     <t>Falta</t>
-  </si>
-  <si>
-    <t>ANDAMENTO</t>
   </si>
 </sst>
 </file>
@@ -804,7 +798,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -922,9 +916,6 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="10" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="25" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2076,10 +2067,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -2399,8 +2386,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="44" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="86" zoomScaleNormal="44" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2423,33 +2410,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="60" t="s">
+      <c r="A1" s="59" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="61"/>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="61"/>
-      <c r="F1" s="61"/>
-      <c r="G1" s="61"/>
-      <c r="H1" s="61"/>
-      <c r="I1" s="61"/>
-      <c r="J1" s="61"/>
-      <c r="K1" s="61"/>
-      <c r="L1" s="61"/>
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="60"/>
+      <c r="F1" s="60"/>
+      <c r="G1" s="60"/>
+      <c r="H1" s="60"/>
+      <c r="I1" s="60"/>
+      <c r="J1" s="60"/>
+      <c r="K1" s="60"/>
+      <c r="L1" s="60"/>
     </row>
     <row r="2" spans="1:17" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="62" t="s">
+      <c r="B2" s="61" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="63"/>
-      <c r="D2" s="62" t="s">
+      <c r="C2" s="62"/>
+      <c r="D2" s="61" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="63"/>
+      <c r="E2" s="62"/>
       <c r="F2" s="1" t="s">
         <v>4</v>
       </c>
@@ -2471,16 +2458,16 @@
       <c r="L2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="N2" s="44"/>
-      <c r="O2" s="45" t="s">
+      <c r="N2" s="43"/>
+      <c r="O2" s="44" t="s">
+        <v>61</v>
+      </c>
+      <c r="P2" s="45" t="s">
         <v>62</v>
-      </c>
-      <c r="P2" s="46" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:17" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="64" t="s">
+      <c r="A3" s="63" t="s">
         <v>11</v>
       </c>
       <c r="B3" s="17">
@@ -2493,67 +2480,67 @@
         <v>1</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G3" s="23" t="s">
         <v>13</v>
       </c>
       <c r="H3" s="18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I3" s="38">
         <v>45967</v>
       </c>
-      <c r="J3" s="43" t="s">
-        <v>61</v>
-      </c>
-      <c r="K3" s="43">
+      <c r="J3" s="42" t="s">
+        <v>60</v>
+      </c>
+      <c r="K3" s="42">
         <v>13</v>
       </c>
-      <c r="L3" s="43">
+      <c r="L3" s="42">
         <v>3</v>
       </c>
-      <c r="N3" s="47" t="s">
-        <v>64</v>
-      </c>
-      <c r="O3" s="48">
+      <c r="N3" s="46" t="s">
+        <v>63</v>
+      </c>
+      <c r="O3" s="47">
         <v>157</v>
       </c>
-      <c r="P3" s="49">
+      <c r="P3" s="48">
         <v>157</v>
       </c>
     </row>
     <row r="4" spans="1:17" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="65"/>
+      <c r="A4" s="64"/>
       <c r="B4" s="17">
         <v>2</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D4" s="2">
         <v>1</v>
       </c>
       <c r="E4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>17</v>
       </c>
       <c r="G4" s="24" t="s">
         <v>13</v>
       </c>
       <c r="H4" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="I4" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="I4" s="38" t="s">
-        <v>19</v>
-      </c>
       <c r="J4" s="21" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K4" s="20">
         <v>8</v>
@@ -2561,235 +2548,245 @@
       <c r="L4" s="4">
         <v>3</v>
       </c>
-      <c r="N4" s="50" t="s">
-        <v>69</v>
-      </c>
-      <c r="O4" s="48">
+      <c r="N4" s="49" t="s">
+        <v>68</v>
+      </c>
+      <c r="O4" s="47">
         <v>0</v>
       </c>
-      <c r="P4" s="49">
+      <c r="P4" s="48">
         <f>SUM(P3-26)</f>
         <v>131</v>
       </c>
     </row>
     <row r="5" spans="1:17" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="66"/>
+      <c r="A5" s="65"/>
       <c r="B5" s="27">
         <v>3</v>
       </c>
       <c r="C5" s="37" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D5" s="35">
         <v>1</v>
       </c>
       <c r="E5" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="34" t="s">
         <v>21</v>
-      </c>
-      <c r="F5" s="34" t="s">
-        <v>22</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>13</v>
       </c>
       <c r="H5" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="I5" s="39"/>
-      <c r="J5" s="43" t="s">
-        <v>58</v>
-      </c>
-      <c r="K5" s="43">
+        <v>17</v>
+      </c>
+      <c r="I5" s="39">
+        <v>45951</v>
+      </c>
+      <c r="J5" s="42" t="s">
+        <v>57</v>
+      </c>
+      <c r="K5" s="42">
         <v>21</v>
       </c>
-      <c r="L5" s="43">
+      <c r="L5" s="42">
         <v>3</v>
       </c>
-      <c r="N5" s="51"/>
-      <c r="O5" s="51"/>
-      <c r="P5" s="51"/>
-      <c r="Q5" s="51"/>
+      <c r="N5" s="50"/>
+      <c r="O5" s="50"/>
+      <c r="P5" s="50"/>
+      <c r="Q5" s="50"/>
     </row>
     <row r="6" spans="1:17" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="76" t="s">
-        <v>23</v>
+      <c r="A6" s="75" t="s">
+        <v>22</v>
       </c>
       <c r="B6" s="28">
         <v>1</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D6" s="6">
         <v>1</v>
       </c>
       <c r="E6" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" s="6" t="s">
         <v>25</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>26</v>
       </c>
       <c r="G6" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="H6" s="42" t="s">
-        <v>14</v>
-      </c>
-      <c r="I6" s="40"/>
-      <c r="J6" s="43" t="s">
-        <v>58</v>
-      </c>
-      <c r="K6" s="43">
+      <c r="H6" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="I6" s="40">
+        <v>45976</v>
+      </c>
+      <c r="J6" s="42" t="s">
+        <v>57</v>
+      </c>
+      <c r="K6" s="42">
         <v>21</v>
       </c>
-      <c r="L6" s="43">
+      <c r="L6" s="42">
         <v>3</v>
       </c>
-      <c r="N6" s="52"/>
-      <c r="O6" s="53"/>
-      <c r="P6" s="52"/>
-      <c r="Q6" s="52"/>
+      <c r="N6" s="51"/>
+      <c r="O6" s="52"/>
+      <c r="P6" s="51"/>
+      <c r="Q6" s="51"/>
     </row>
     <row r="7" spans="1:17" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="77"/>
-      <c r="B7" s="79">
+      <c r="A7" s="76"/>
+      <c r="B7" s="78">
         <v>2</v>
       </c>
-      <c r="C7" s="81" t="s">
-        <v>27</v>
+      <c r="C7" s="80" t="s">
+        <v>26</v>
       </c>
       <c r="D7" s="6">
         <v>1</v>
       </c>
       <c r="E7" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F7" s="6" t="s">
         <v>28</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>29</v>
       </c>
       <c r="G7" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="H7" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="I7" s="38"/>
-      <c r="J7" s="43" t="s">
-        <v>59</v>
-      </c>
-      <c r="K7" s="43">
+      <c r="H7" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="I7" s="38">
+        <v>45979</v>
+      </c>
+      <c r="J7" s="42" t="s">
+        <v>58</v>
+      </c>
+      <c r="K7" s="42">
         <v>8</v>
       </c>
-      <c r="L7" s="43">
+      <c r="L7" s="42">
         <v>3</v>
       </c>
-      <c r="N7" s="54"/>
-      <c r="O7" s="54"/>
-      <c r="P7" s="52"/>
-      <c r="Q7" s="52"/>
+      <c r="N7" s="53"/>
+      <c r="O7" s="53"/>
+      <c r="P7" s="51"/>
+      <c r="Q7" s="51"/>
     </row>
     <row r="8" spans="1:17" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="78"/>
-      <c r="B8" s="80"/>
-      <c r="C8" s="82"/>
+      <c r="A8" s="77"/>
+      <c r="B8" s="79"/>
+      <c r="C8" s="81"/>
       <c r="D8" s="6">
         <v>2</v>
       </c>
       <c r="E8" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F8" s="6" t="s">
         <v>30</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>31</v>
       </c>
       <c r="G8" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="H8" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="I8" s="38"/>
-      <c r="J8" s="43" t="s">
-        <v>59</v>
-      </c>
-      <c r="K8" s="43">
+      <c r="H8" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="I8" s="38">
+        <v>45979</v>
+      </c>
+      <c r="J8" s="42" t="s">
+        <v>58</v>
+      </c>
+      <c r="K8" s="42">
         <v>8</v>
       </c>
-      <c r="L8" s="43">
+      <c r="L8" s="42">
         <v>3</v>
       </c>
-      <c r="N8" s="54"/>
-      <c r="O8" s="54"/>
-      <c r="P8" s="54"/>
-      <c r="Q8" s="54"/>
+      <c r="N8" s="53"/>
+      <c r="O8" s="53"/>
+      <c r="P8" s="53"/>
+      <c r="Q8" s="53"/>
     </row>
     <row r="9" spans="1:17" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="74" t="s">
-        <v>32</v>
+      <c r="A9" s="73" t="s">
+        <v>31</v>
       </c>
       <c r="B9" s="29">
         <v>1</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D9" s="8">
         <v>1</v>
       </c>
       <c r="E9" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="F9" s="8" t="s">
         <v>34</v>
-      </c>
-      <c r="F9" s="8" t="s">
-        <v>35</v>
       </c>
       <c r="G9" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="H9" s="18" t="s">
-        <v>18</v>
+      <c r="H9" s="19" t="s">
+        <v>17</v>
       </c>
       <c r="I9" s="38">
         <v>45668</v>
       </c>
-      <c r="J9" s="43" t="s">
-        <v>60</v>
-      </c>
-      <c r="K9" s="43">
+      <c r="J9" s="42" t="s">
+        <v>59</v>
+      </c>
+      <c r="K9" s="42">
         <v>5</v>
       </c>
-      <c r="L9" s="43">
+      <c r="L9" s="42">
         <v>2</v>
       </c>
-      <c r="N9" s="54"/>
-      <c r="O9" s="54"/>
-      <c r="P9" s="54"/>
-      <c r="Q9" s="54"/>
+      <c r="N9" s="53"/>
+      <c r="O9" s="53"/>
+      <c r="P9" s="53"/>
+      <c r="Q9" s="53"/>
     </row>
     <row r="10" spans="1:17" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="75"/>
+      <c r="A10" s="74"/>
       <c r="B10" s="29">
         <v>2</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D10" s="8">
         <v>1</v>
       </c>
       <c r="E10" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="F10" s="8" t="s">
         <v>37</v>
-      </c>
-      <c r="F10" s="8" t="s">
-        <v>38</v>
       </c>
       <c r="G10" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="H10" s="18" t="s">
-        <v>70</v>
-      </c>
-      <c r="I10" s="38"/>
+      <c r="H10" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="I10" s="38">
+        <v>45967</v>
+      </c>
       <c r="J10" s="20" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K10" s="20">
         <v>5</v>
@@ -2797,248 +2794,258 @@
       <c r="L10" s="4">
         <v>2</v>
       </c>
-      <c r="N10" s="54"/>
-      <c r="O10" s="54"/>
-      <c r="P10" s="54"/>
-      <c r="Q10" s="54"/>
+      <c r="N10" s="53"/>
+      <c r="O10" s="53"/>
+      <c r="P10" s="53"/>
+      <c r="Q10" s="53"/>
     </row>
     <row r="11" spans="1:17" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="67" t="s">
+      <c r="A11" s="66" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" s="71">
+        <v>1</v>
+      </c>
+      <c r="C11" s="69" t="s">
         <v>39</v>
-      </c>
-      <c r="B11" s="72">
-        <v>1</v>
-      </c>
-      <c r="C11" s="70" t="s">
-        <v>40</v>
       </c>
       <c r="D11" s="10">
         <v>1</v>
       </c>
       <c r="E11" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="F11" s="10" t="s">
         <v>41</v>
-      </c>
-      <c r="F11" s="10" t="s">
-        <v>42</v>
       </c>
       <c r="G11" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="H11" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="I11" s="38"/>
-      <c r="J11" s="43" t="s">
-        <v>61</v>
-      </c>
-      <c r="K11" s="43">
+      <c r="H11" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="I11" s="38">
+        <v>45977</v>
+      </c>
+      <c r="J11" s="42" t="s">
+        <v>60</v>
+      </c>
+      <c r="K11" s="42">
         <v>13</v>
       </c>
-      <c r="L11" s="43">
+      <c r="L11" s="42">
         <v>2</v>
       </c>
-      <c r="N11" s="54"/>
-      <c r="O11" s="54"/>
-      <c r="P11" s="54"/>
-      <c r="Q11" s="54"/>
+      <c r="N11" s="53"/>
+      <c r="O11" s="53"/>
+      <c r="P11" s="53"/>
+      <c r="Q11" s="53"/>
     </row>
     <row r="12" spans="1:17" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="68"/>
-      <c r="B12" s="73"/>
-      <c r="C12" s="71"/>
+      <c r="A12" s="67"/>
+      <c r="B12" s="72"/>
+      <c r="C12" s="70"/>
       <c r="D12" s="10">
         <v>2</v>
       </c>
       <c r="E12" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="F12" s="10" t="s">
         <v>43</v>
-      </c>
-      <c r="F12" s="10" t="s">
-        <v>44</v>
       </c>
       <c r="G12" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="H12" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="I12" s="38"/>
-      <c r="J12" s="43" t="s">
-        <v>61</v>
-      </c>
-      <c r="K12" s="43">
+      <c r="H12" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="I12" s="38">
+        <v>45977</v>
+      </c>
+      <c r="J12" s="42" t="s">
+        <v>60</v>
+      </c>
+      <c r="K12" s="42">
         <v>13</v>
       </c>
-      <c r="L12" s="43">
+      <c r="L12" s="42">
         <v>2</v>
       </c>
-      <c r="N12" s="54"/>
-      <c r="O12" s="54"/>
-      <c r="P12" s="54"/>
-      <c r="Q12" s="54"/>
+      <c r="N12" s="53"/>
+      <c r="O12" s="53"/>
+      <c r="P12" s="53"/>
+      <c r="Q12" s="53"/>
     </row>
     <row r="13" spans="1:17" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="69"/>
+      <c r="A13" s="68"/>
       <c r="B13" s="30">
         <v>2</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D13" s="10">
         <v>1</v>
       </c>
       <c r="E13" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="F13" s="10" t="s">
         <v>46</v>
-      </c>
-      <c r="F13" s="10" t="s">
-        <v>47</v>
       </c>
       <c r="G13" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="H13" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="I13" s="41"/>
-      <c r="J13" s="43" t="s">
-        <v>58</v>
-      </c>
-      <c r="K13" s="43">
+      <c r="H13" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="I13" s="41">
+        <v>45977</v>
+      </c>
+      <c r="J13" s="42" t="s">
+        <v>57</v>
+      </c>
+      <c r="K13" s="42">
         <v>21</v>
       </c>
-      <c r="L13" s="43">
+      <c r="L13" s="42">
         <v>3</v>
       </c>
-      <c r="N13" s="54"/>
-      <c r="O13" s="54"/>
-      <c r="P13" s="54"/>
-      <c r="Q13" s="54"/>
+      <c r="N13" s="53"/>
+      <c r="O13" s="53"/>
+      <c r="P13" s="53"/>
+      <c r="Q13" s="53"/>
     </row>
     <row r="14" spans="1:17" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B14" s="31">
         <v>1</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D14" s="12">
         <v>1</v>
       </c>
       <c r="E14" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="F14" s="12" t="s">
         <v>50</v>
-      </c>
-      <c r="F14" s="12" t="s">
-        <v>51</v>
       </c>
       <c r="G14" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="H14" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="I14" s="41"/>
-      <c r="J14" s="43" t="s">
-        <v>59</v>
-      </c>
-      <c r="K14" s="43">
+      <c r="H14" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="I14" s="41">
+        <v>45976</v>
+      </c>
+      <c r="J14" s="42" t="s">
+        <v>58</v>
+      </c>
+      <c r="K14" s="42">
         <v>8</v>
       </c>
-      <c r="L14" s="43">
+      <c r="L14" s="42">
         <v>2</v>
       </c>
-      <c r="N14" s="54"/>
-      <c r="O14" s="54"/>
-      <c r="P14" s="54"/>
-      <c r="Q14" s="54"/>
+      <c r="N14" s="53"/>
+      <c r="O14" s="53"/>
+      <c r="P14" s="53"/>
+      <c r="Q14" s="53"/>
     </row>
     <row r="15" spans="1:17" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="16" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B15" s="32">
         <v>1</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D15" s="14">
         <v>1</v>
       </c>
       <c r="E15" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="F15" s="14" t="s">
         <v>54</v>
-      </c>
-      <c r="F15" s="14" t="s">
-        <v>55</v>
       </c>
       <c r="G15" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="H15" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="I15" s="41"/>
-      <c r="J15" s="43" t="s">
-        <v>61</v>
-      </c>
-      <c r="K15" s="43">
+      <c r="H15" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="I15" s="41">
+        <v>45984</v>
+      </c>
+      <c r="J15" s="42" t="s">
+        <v>60</v>
+      </c>
+      <c r="K15" s="42">
         <v>13</v>
       </c>
-      <c r="L15" s="43">
+      <c r="L15" s="42">
         <v>2</v>
       </c>
-      <c r="N15" s="54"/>
-      <c r="O15" s="54"/>
-      <c r="P15" s="54"/>
-      <c r="Q15" s="54"/>
+      <c r="N15" s="53"/>
+      <c r="O15" s="53"/>
+      <c r="P15" s="53"/>
+      <c r="Q15" s="53"/>
     </row>
     <row r="16" spans="1:17" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="I16" s="25"/>
       <c r="J16" s="26"/>
-      <c r="N16" s="54"/>
-      <c r="O16" s="54"/>
-      <c r="Q16" s="54"/>
+      <c r="N16" s="53"/>
+      <c r="O16" s="53"/>
+      <c r="Q16" s="53"/>
     </row>
     <row r="17" spans="8:17" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="J17" s="57" t="s">
-        <v>65</v>
-      </c>
-      <c r="K17" s="58"/>
-      <c r="L17" s="59"/>
-      <c r="N17" s="54"/>
-      <c r="O17" s="54"/>
-      <c r="P17" s="54"/>
-      <c r="Q17" s="54"/>
+      <c r="J17" s="56" t="s">
+        <v>64</v>
+      </c>
+      <c r="K17" s="57"/>
+      <c r="L17" s="58"/>
+      <c r="N17" s="53"/>
+      <c r="O17" s="53"/>
+      <c r="P17" s="53"/>
+      <c r="Q17" s="53"/>
     </row>
     <row r="18" spans="8:17" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H18" s="36"/>
-      <c r="J18" s="50" t="s">
+      <c r="J18" s="49" t="s">
+        <v>65</v>
+      </c>
+      <c r="K18" s="49" t="s">
         <v>66</v>
       </c>
-      <c r="K18" s="50" t="s">
+      <c r="L18" s="49" t="s">
         <v>67</v>
       </c>
-      <c r="L18" s="50" t="s">
-        <v>68</v>
-      </c>
-      <c r="N18" s="54"/>
-      <c r="O18" s="54"/>
-      <c r="P18" s="54"/>
-      <c r="Q18" s="54"/>
+      <c r="N18" s="53"/>
+      <c r="O18" s="53"/>
+      <c r="P18" s="53"/>
+      <c r="Q18" s="53"/>
     </row>
     <row r="19" spans="8:17" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="N19" s="54"/>
-      <c r="O19" s="55"/>
-      <c r="P19" s="55"/>
-      <c r="Q19" s="55"/>
+      <c r="N19" s="53"/>
+      <c r="O19" s="54"/>
+      <c r="P19" s="54"/>
+      <c r="Q19" s="54"/>
     </row>
     <row r="20" spans="8:17" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="N20" s="56"/>
+      <c r="N20" s="55"/>
     </row>
     <row r="21" spans="8:17" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="N21" s="56"/>
+      <c r="N21" s="55"/>
     </row>
   </sheetData>
   <mergeCells count="12">

</xml_diff>